<commit_message>
rename icon folders add colors to actions add file names to actions add icons to nodes add people icons add new icons to nodes
</commit_message>
<xml_diff>
--- a/data/exported_python/graph_reduced.xlsx
+++ b/data/exported_python/graph_reduced.xlsx
@@ -3497,7 +3497,7 @@
         </is>
       </c>
       <c r="D101" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E101" t="n">
         <v>17</v>
@@ -3510,7 +3510,7 @@
         <v>7</v>
       </c>
       <c r="I101" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="102">
@@ -3526,7 +3526,7 @@
         </is>
       </c>
       <c r="D102" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E102" t="n">
         <v>17</v>
@@ -3539,7 +3539,7 @@
         <v>9</v>
       </c>
       <c r="I102" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="103">
@@ -3555,7 +3555,7 @@
         </is>
       </c>
       <c r="D103" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E103" t="n">
         <v>17</v>
@@ -3568,7 +3568,7 @@
         <v>10</v>
       </c>
       <c r="I103" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="104">
@@ -3584,7 +3584,7 @@
         </is>
       </c>
       <c r="D104" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E104" t="n">
         <v>17</v>
@@ -3597,7 +3597,7 @@
         <v>15</v>
       </c>
       <c r="I104" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="105">
@@ -3613,7 +3613,7 @@
         </is>
       </c>
       <c r="D105" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E105" t="n">
         <v>17</v>
@@ -3626,7 +3626,7 @@
         <v>18</v>
       </c>
       <c r="I105" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="106">
@@ -3642,7 +3642,7 @@
         </is>
       </c>
       <c r="D106" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E106" t="n">
         <v>17</v>
@@ -3655,7 +3655,7 @@
         <v>19</v>
       </c>
       <c r="I106" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="107">
@@ -3671,7 +3671,7 @@
         </is>
       </c>
       <c r="D107" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E107" t="n">
         <v>17</v>
@@ -3684,7 +3684,7 @@
         <v>21</v>
       </c>
       <c r="I107" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="108">
@@ -3700,7 +3700,7 @@
         </is>
       </c>
       <c r="D108" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E108" t="n">
         <v>17</v>
@@ -3713,7 +3713,7 @@
         <v>22</v>
       </c>
       <c r="I108" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="109">
@@ -3729,7 +3729,7 @@
         </is>
       </c>
       <c r="D109" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E109" t="n">
         <v>17</v>
@@ -3742,7 +3742,7 @@
         <v>23</v>
       </c>
       <c r="I109" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="110">
@@ -3758,7 +3758,7 @@
         </is>
       </c>
       <c r="D110" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E110" t="n">
         <v>17</v>
@@ -3771,7 +3771,7 @@
         <v>24</v>
       </c>
       <c r="I110" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="111">
@@ -3787,7 +3787,7 @@
         </is>
       </c>
       <c r="D111" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E111" t="n">
         <v>17</v>
@@ -3800,7 +3800,7 @@
         <v>25</v>
       </c>
       <c r="I111" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="112">
@@ -3816,7 +3816,7 @@
         </is>
       </c>
       <c r="D112" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E112" t="n">
         <v>17</v>
@@ -3829,7 +3829,7 @@
         <v>26</v>
       </c>
       <c r="I112" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="113">
@@ -3845,7 +3845,7 @@
         </is>
       </c>
       <c r="D113" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E113" t="n">
         <v>17</v>
@@ -3858,7 +3858,7 @@
         <v>29</v>
       </c>
       <c r="I113" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="114">
@@ -3874,7 +3874,7 @@
         </is>
       </c>
       <c r="D114" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E114" t="n">
         <v>17</v>
@@ -3887,7 +3887,7 @@
         <v>31</v>
       </c>
       <c r="I114" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="115">
@@ -3903,7 +3903,7 @@
         </is>
       </c>
       <c r="D115" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E115" t="n">
         <v>17</v>
@@ -3916,7 +3916,7 @@
         <v>35</v>
       </c>
       <c r="I115" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="116">

</xml_diff>